<commit_message>
groupDetails work about 70% complete for css
</commit_message>
<xml_diff>
--- a/public/excel_docs/masterDoc.xlsx
+++ b/public/excel_docs/masterDoc.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joseph.collins/Documents/personal-projects/world-cup/world-cup-friends/public/excel_docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4309F083-3D93-0042-A8D9-E6A573AF6CF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8537DF9B-604E-4A4E-8F23-271B5BB5E841}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34600" yWindow="560" windowWidth="29280" windowHeight="20560" activeTab="5" xr2:uid="{936879F1-3B23-4C40-8D99-B1D384C793DF}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19860" activeTab="5" xr2:uid="{936879F1-3B23-4C40-8D99-B1D384C793DF}"/>
   </bookViews>
   <sheets>
     <sheet name="results_MASTER" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="joe-stan" sheetId="2" r:id="rId3"/>
     <sheet name="kelly" sheetId="5" r:id="rId4"/>
     <sheet name="coach" sheetId="6" r:id="rId5"/>
-    <sheet name="kevin" sheetId="8" r:id="rId6"/>
+    <sheet name="aboona" sheetId="8" r:id="rId6"/>
     <sheet name="templateUser" sheetId="7" r:id="rId7"/>
   </sheets>
   <definedNames>
@@ -6805,7 +6805,7 @@
   <dimension ref="A1:S25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F33" sqref="F33"/>
+      <selection activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7186,14 +7186,14 @@
       <c r="C12" s="25"/>
       <c r="D12" s="26"/>
       <c r="E12" s="38"/>
-      <c r="F12" s="22" t="s">
+      <c r="F12" s="24" t="s">
         <v>39</v>
       </c>
       <c r="G12" s="25"/>
       <c r="H12" s="25"/>
       <c r="I12" s="26"/>
       <c r="J12" s="38"/>
-      <c r="K12" s="22" t="s">
+      <c r="K12" s="24" t="s">
         <v>54</v>
       </c>
       <c r="L12" s="25"/>
@@ -7207,7 +7207,7 @@
       <c r="R12" s="25"/>
       <c r="S12" s="26"/>
     </row>
-    <row r="13" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A13" s="8" t="s">
         <v>16</v>
       </c>
@@ -7215,14 +7215,14 @@
       <c r="C13" s="4"/>
       <c r="D13" s="27"/>
       <c r="E13" s="38"/>
-      <c r="F13" s="22" t="s">
+      <c r="F13" s="8" t="s">
         <v>36</v>
       </c>
       <c r="G13" s="4"/>
       <c r="H13" s="4"/>
       <c r="I13" s="27"/>
       <c r="J13" s="38"/>
-      <c r="K13" s="22" t="s">
+      <c r="K13" s="8" t="s">
         <v>57</v>
       </c>
       <c r="L13" s="4"/>
@@ -7236,7 +7236,7 @@
       <c r="R13" s="4"/>
       <c r="S13" s="27"/>
     </row>
-    <row r="14" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A14" s="8" t="s">
         <v>14</v>
       </c>
@@ -7246,14 +7246,14 @@
       </c>
       <c r="D14" s="27"/>
       <c r="E14" s="38"/>
-      <c r="F14" s="23" t="s">
+      <c r="F14" s="8" t="s">
         <v>37</v>
       </c>
       <c r="G14" s="4"/>
       <c r="H14" s="4"/>
       <c r="I14" s="27"/>
       <c r="J14" s="38"/>
-      <c r="K14" s="21" t="s">
+      <c r="K14" s="8" t="s">
         <v>56</v>
       </c>
       <c r="L14" s="4"/>
@@ -7279,14 +7279,14 @@
       <c r="C15" s="28"/>
       <c r="D15" s="29"/>
       <c r="E15" s="38"/>
-      <c r="F15" s="21" t="s">
+      <c r="F15" s="10" t="s">
         <v>38</v>
       </c>
       <c r="G15" s="28"/>
       <c r="H15" s="28"/>
       <c r="I15" s="29"/>
       <c r="J15" s="38"/>
-      <c r="K15" s="23" t="s">
+      <c r="K15" s="10" t="s">
         <v>55</v>
       </c>
       <c r="L15" s="28"/>
@@ -7909,7 +7909,7 @@
   <dimension ref="A1:S25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G36" sqref="G36"/>
+      <selection activeCell="I35" sqref="I35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>